<commit_message>
defined 'save_questions_to_db' function in 'database_communication' class
</commit_message>
<xml_diff>
--- a/data/questions_and_choices.xlsx
+++ b/data/questions_and_choices.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t xml:space="preserve">NO.</t>
   </si>
@@ -77,6 +77,45 @@
   </si>
   <si>
     <t xml:space="preserve">زبان</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how old are you?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not important</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it’s none of your buisiness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who the hell would have cared?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get lost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it’s not important</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how big is earth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.esri.com/news/arcuser/0610/graphics/nospin_1-lg.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who is an old guy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/5/53/Random_Old_Guy.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://jooinn.com/images/happy-young-man-1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.stockvault.net/data/2018/04/25/250732/preview16.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://d2v9y0dukr6mq2.cloudfront.net/video/thumbnail/NGyZeGzFlijx95hou/4k-close-up-face-of-a-young-man-without-emotions-beautiful-frowning-guy-in-a-white-shirt-looking-to-the-camera_bjv1icufl_thumbnail-full01.png</t>
   </si>
 </sst>
 </file>
@@ -91,6 +130,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -111,6 +151,7 @@
       <sz val="10"/>
       <name val="Lohit Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -181,10 +222,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -270,6 +311,84 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>85000</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
first prototype of the project
</commit_message>
<xml_diff>
--- a/data/questions_and_choices.xlsx
+++ b/data/questions_and_choices.xlsx
@@ -5,10 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="questions_and_choices" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="daily" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="psychology" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="sport" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="cooking" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="electrical_engineering" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="80">
   <si>
     <t xml:space="preserve">NO.</t>
   </si>
@@ -116,6 +120,168 @@
   </si>
   <si>
     <t xml:space="preserve">https://d2v9y0dukr6mq2.cloudfront.net/video/thumbnail/NGyZeGzFlijx95hou/4k-close-up-face-of-a-young-man-without-emotions-beautiful-frowning-guy-in-a-white-shirt-looking-to-the-camera_bjv1icufl_thumbnail-full01.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who is mad?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://amp.businessinsider.com/images/5c4388312bdd7f10b33a8345-750-375.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://i.pinimg.com/originals/27/72/da/2772da69c3efb96881850a48f87c287a.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Jfk2.jpg/1200px-Jfk2.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/8/8d/President_Barack_Obama.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who was the winner of the world heavyweight championship in 1964</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mike tyson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sonny liston</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cassius Clay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frank Bruno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">who’s the owner of the quote “Float Like A Butterfly, Sting Like A Bee”?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elvis Presley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Willie Nelson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vladimir Putin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what was the religion of muhamad ali clay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muslim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jewish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">christian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn.cnn.com/cnnnext/dam/assets/160428123740-muhammad-ali-7-large-169.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How many times did Muhammad Ali win the heavyweight title?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">three times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">two times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">once</t>
+  </si>
+  <si>
+    <t xml:space="preserve">five times</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cdn-s3.si.com/s3fs-public/styles/marquee_large_2x/public/videos/2157889318001_4250021492001_ali.jpg?itok=UdA7p09r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مخترع دستگاه ام ار ای که بود؟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ریموند دامادین</t>
+  </si>
+  <si>
+    <t xml:space="preserve">لویی باستور</t>
+  </si>
+  <si>
+    <t xml:space="preserve">فردریک لاتربور</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آنتوان لاوازیه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.liberty.edu/wwwadmin/images/v4template/news/damadian-portrait-1luh_792.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ایده دستگاه ام ار ای از چه دستگاهی بود؟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ان ام ار</t>
+  </si>
+  <si>
+    <t xml:space="preserve">سیتی اسکن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">رادیولوژی</t>
+  </si>
+  <si>
+    <t xml:space="preserve">قفس فاراده</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">https://www.newskarnataka</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.com/news-inner-images/mri_ms_child_newsk_88252053.jpeg</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">تصویر برداری دستگاه ام ار ای بر چه اساس انجام میشود؟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">آب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بروتون های مولکول های هیدروژن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">الکترون های اکسیژن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">چربی موجود در بدن</t>
+  </si>
+  <si>
+    <t xml:space="preserve">به واحد های تشکیل دهنده تصاویر ام ار ای چه نام دارد؟</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بیکسل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ماتریس</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ولوم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">واکسل</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://assets.aboutkidshealth.ca/akhassets/BT_Neuro_MRI2_MEDIMG-PHO_EN.jpg?RenditionID=10</t>
   </si>
 </sst>
 </file>
@@ -125,7 +291,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -150,6 +316,13 @@
     <font>
       <sz val="10"/>
       <name val="Lohit Devanagari"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -196,12 +369,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -224,8 +409,8 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -398,4 +583,461 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="https://upload.wikimedia.org/wikipedia/commons/thumb/7/70/Jfk2.jpg/1200px-Jfk2.jpg"/>
+    <hyperlink ref="F2" r:id="rId2" display="https://upload.wikimedia.org/wikipedia/commons/8/8d/President_Barack_Obama.jpg"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H4" r:id="rId1" display="https://cdn.cnn.com/cnnnext/dam/assets/160428123740-muhammad-ali-7-large-169.jpg"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" display="https://www.newskarnataka"/>
+    <hyperlink ref="H5" r:id="rId2" display="https://assets.aboutkidshealth.ca/akhassets/BT_Neuro_MRI2_MEDIMG-PHO_EN.jpg?RenditionID=10"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>